<commit_message>
P05 Option, Customer, Computer
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="147">
   <si>
     <t>Product Name:</t>
   </si>
@@ -479,6 +479,9 @@
   </si>
   <si>
     <t>Completed Day 4</t>
+  </si>
+  <si>
+    <t>Write Computer Class Aggregation</t>
   </si>
 </sst>
 </file>
@@ -870,6 +873,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1012,11 +1016,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209233304"/>
-        <c:axId val="114869968"/>
+        <c:axId val="189038160"/>
+        <c:axId val="189043256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="209233304"/>
+        <c:axId val="189038160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1044,6 +1048,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1075,12 +1080,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114869968"/>
+        <c:crossAx val="189043256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="114869968"/>
+        <c:axId val="189043256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1116,6 +1121,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1147,7 +1153,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209233304"/>
+        <c:crossAx val="189038160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1278,28 +1284,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1327,11 +1333,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="209186664"/>
-        <c:axId val="209187048"/>
+        <c:axId val="189041688"/>
+        <c:axId val="189044040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209186664"/>
+        <c:axId val="189041688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,7 +1395,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209187048"/>
+        <c:crossAx val="189044040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1397,7 +1403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209187048"/>
+        <c:axId val="189044040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1464,7 +1470,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209186664"/>
+        <c:crossAx val="189041688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1643,11 +1649,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="208819144"/>
-        <c:axId val="208822672"/>
+        <c:axId val="189042864"/>
+        <c:axId val="189040904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208819144"/>
+        <c:axId val="189042864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1704,7 +1710,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208822672"/>
+        <c:crossAx val="189040904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1712,7 +1718,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208822672"/>
+        <c:axId val="189040904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1778,7 +1784,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208819144"/>
+        <c:crossAx val="189042864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1957,11 +1963,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="208818752"/>
-        <c:axId val="208826200"/>
+        <c:axId val="189037768"/>
+        <c:axId val="189040120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208818752"/>
+        <c:axId val="189037768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2018,7 +2024,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208826200"/>
+        <c:crossAx val="189040120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2026,7 +2032,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208826200"/>
+        <c:axId val="189040120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2092,7 +2098,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208818752"/>
+        <c:crossAx val="189037768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2271,11 +2277,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="208821104"/>
-        <c:axId val="208825024"/>
+        <c:axId val="189037376"/>
+        <c:axId val="209284080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208821104"/>
+        <c:axId val="189037376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2332,7 +2338,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208825024"/>
+        <c:crossAx val="209284080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2340,7 +2346,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208825024"/>
+        <c:axId val="209284080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2406,7 +2412,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208821104"/>
+        <c:crossAx val="189037376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2585,11 +2591,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="208821496"/>
-        <c:axId val="208822280"/>
+        <c:axId val="209285256"/>
+        <c:axId val="209287608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208821496"/>
+        <c:axId val="209285256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2646,7 +2652,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208822280"/>
+        <c:crossAx val="209287608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2654,7 +2660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208822280"/>
+        <c:axId val="209287608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2720,7 +2726,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208821496"/>
+        <c:crossAx val="209285256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2899,11 +2905,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="209239216"/>
-        <c:axId val="209240000"/>
+        <c:axId val="209289176"/>
+        <c:axId val="209288000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209239216"/>
+        <c:axId val="209289176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2960,7 +2966,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209240000"/>
+        <c:crossAx val="209288000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2968,7 +2974,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209240000"/>
+        <c:axId val="209288000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3034,7 +3040,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209239216"/>
+        <c:crossAx val="209289176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3087,7 +3093,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3128,7 +3134,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3169,7 +3175,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3210,7 +3216,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3251,7 +3257,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3292,7 +3298,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3333,7 +3339,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3656,8 +3662,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4122,7 +4128,9 @@
       <c r="F25" s="17">
         <v>1</v>
       </c>
-      <c r="G25" s="17"/>
+      <c r="G25" s="17" t="s">
+        <v>138</v>
+      </c>
       <c r="H25" s="18" t="s">
         <v>36</v>
       </c>
@@ -5406,8 +5414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5510,7 +5518,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5525,7 +5533,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5543,7 +5551,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5561,7 +5569,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5579,11 +5587,11 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -5597,7 +5605,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5615,7 +5623,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5633,7 +5641,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -5775,21 +5783,35 @@
       <c r="A23" s="1">
         <v>7</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="35" t="s">
+        <v>30</v>
+      </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="37"/>
+      <c r="D23" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>138</v>
+      </c>
       <c r="F23" s="38"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>8</v>
       </c>
-      <c r="B24" s="35"/>
+      <c r="B24" s="35" t="s">
+        <v>30</v>
+      </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="38"/>
+      <c r="D24" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="F24" s="38" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">

</xml_diff>

<commit_message>
P05 Option, Customer, Computer TrialRun
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="148">
   <si>
     <t>Product Name:</t>
   </si>
@@ -482,6 +482,9 @@
   </si>
   <si>
     <t>Write Computer Class Aggregation</t>
+  </si>
+  <si>
+    <t>Add Customer, Option, &amp; Computer to GitHub</t>
   </si>
 </sst>
 </file>
@@ -873,7 +876,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1016,11 +1018,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189038160"/>
-        <c:axId val="189043256"/>
+        <c:axId val="115147032"/>
+        <c:axId val="40016200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189038160"/>
+        <c:axId val="115147032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1048,7 +1050,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1080,12 +1081,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189043256"/>
+        <c:crossAx val="40016200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189043256"/>
+        <c:axId val="40016200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1121,7 +1122,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1153,7 +1153,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189038160"/>
+        <c:crossAx val="115147032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1284,16 +1284,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>4</c:v>
@@ -1333,11 +1333,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="189041688"/>
-        <c:axId val="189044040"/>
+        <c:axId val="207391352"/>
+        <c:axId val="207392920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189041688"/>
+        <c:axId val="207391352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1395,7 +1395,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189044040"/>
+        <c:crossAx val="207392920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1403,7 +1403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189044040"/>
+        <c:axId val="207392920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1470,7 +1470,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189041688"/>
+        <c:crossAx val="207391352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1649,11 +1649,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="189042864"/>
-        <c:axId val="189040904"/>
+        <c:axId val="207392136"/>
+        <c:axId val="207389000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189042864"/>
+        <c:axId val="207392136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1710,7 +1710,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189040904"/>
+        <c:crossAx val="207389000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1718,7 +1718,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189040904"/>
+        <c:axId val="207389000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1784,7 +1784,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189042864"/>
+        <c:crossAx val="207392136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1963,11 +1963,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="189037768"/>
-        <c:axId val="189040120"/>
+        <c:axId val="207393312"/>
+        <c:axId val="207394488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189037768"/>
+        <c:axId val="207393312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2024,7 +2024,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189040120"/>
+        <c:crossAx val="207394488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2032,7 +2032,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189040120"/>
+        <c:axId val="207394488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2098,7 +2098,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189037768"/>
+        <c:crossAx val="207393312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2277,11 +2277,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="189037376"/>
-        <c:axId val="209284080"/>
+        <c:axId val="207391744"/>
+        <c:axId val="207390568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189037376"/>
+        <c:axId val="207391744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2338,7 +2338,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209284080"/>
+        <c:crossAx val="207390568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2346,7 +2346,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209284080"/>
+        <c:axId val="207390568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2412,7 +2412,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189037376"/>
+        <c:crossAx val="207391744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2591,11 +2591,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="209285256"/>
-        <c:axId val="209287608"/>
+        <c:axId val="208758744"/>
+        <c:axId val="208754824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209285256"/>
+        <c:axId val="208758744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2652,7 +2652,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209287608"/>
+        <c:crossAx val="208754824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2660,7 +2660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209287608"/>
+        <c:axId val="208754824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2726,7 +2726,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209285256"/>
+        <c:crossAx val="208758744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2905,11 +2905,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="209289176"/>
-        <c:axId val="209288000"/>
+        <c:axId val="208755608"/>
+        <c:axId val="208759528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209289176"/>
+        <c:axId val="208755608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2966,7 +2966,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209288000"/>
+        <c:crossAx val="208759528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2974,7 +2974,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209288000"/>
+        <c:axId val="208759528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3040,7 +3040,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209289176"/>
+        <c:crossAx val="208755608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3093,7 +3093,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3134,7 +3134,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3175,7 +3175,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3216,7 +3216,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3257,7 +3257,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3298,7 +3298,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3339,7 +3339,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5414,7 +5414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -5518,7 +5518,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5533,7 +5533,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5569,7 +5569,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5591,7 +5591,7 @@
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -5804,7 +5804,7 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="39" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E24" s="37" t="s">
         <v>145</v>
@@ -5817,11 +5817,19 @@
       <c r="A25" s="1">
         <v>9</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="35" t="s">
+        <v>30</v>
+      </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="38"/>
+      <c r="D25" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="F25" s="38" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">

</xml_diff>

<commit_message>
P05 Order & Computer Rev
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="152">
   <si>
     <t>Product Name:</t>
   </si>
@@ -494,6 +494,9 @@
   </si>
   <si>
     <t>Completed Day 5</t>
+  </si>
+  <si>
+    <t>Add Order &amp; Computer revisions to GitHub</t>
   </si>
 </sst>
 </file>
@@ -1295,19 +1298,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
@@ -5426,7 +5429,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5529,7 +5532,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5544,7 +5547,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5562,7 +5565,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5580,7 +5583,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5598,7 +5601,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5620,7 +5623,7 @@
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -5880,10 +5883,16 @@
       <c r="A28" s="1">
         <v>12</v>
       </c>
-      <c r="B28" s="35"/>
+      <c r="B28" s="35" t="s">
+        <v>43</v>
+      </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="37"/>
+      <c r="D28" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>150</v>
+      </c>
       <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
P05 Add Customer REGEX revisions to GitHub
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="156">
   <si>
     <t>Product Name:</t>
   </si>
@@ -500,6 +500,15 @@
   </si>
   <si>
     <t>Add Customer revisions to to GitHub</t>
+  </si>
+  <si>
+    <t>Write Customer class REGEX</t>
+  </si>
+  <si>
+    <t>Completed Day 6</t>
+  </si>
+  <si>
+    <t>Add Customer REGEX revisions to GitHub</t>
   </si>
 </sst>
 </file>
@@ -1033,11 +1042,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="208720744"/>
-        <c:axId val="208714080"/>
+        <c:axId val="222334448"/>
+        <c:axId val="222331704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="208720744"/>
+        <c:axId val="222334448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1096,12 +1105,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208714080"/>
+        <c:crossAx val="222331704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="208714080"/>
+        <c:axId val="222331704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1168,7 +1177,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208720744"/>
+        <c:crossAx val="222334448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1298,22 +1307,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5</c:v>
@@ -1347,11 +1356,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="208719568"/>
-        <c:axId val="208719960"/>
+        <c:axId val="222332096"/>
+        <c:axId val="222332880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208719568"/>
+        <c:axId val="222332096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1408,7 +1417,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208719960"/>
+        <c:crossAx val="222332880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1416,7 +1425,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208719960"/>
+        <c:axId val="222332880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1482,7 +1491,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208719568"/>
+        <c:crossAx val="222332096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1661,11 +1670,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="208718000"/>
-        <c:axId val="208714864"/>
+        <c:axId val="222331312"/>
+        <c:axId val="222333664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208718000"/>
+        <c:axId val="222331312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1722,7 +1731,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208714864"/>
+        <c:crossAx val="222333664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1730,7 +1739,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208714864"/>
+        <c:axId val="222333664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1796,7 +1805,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208718000"/>
+        <c:crossAx val="222331312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1975,11 +1984,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="208716432"/>
-        <c:axId val="208715256"/>
+        <c:axId val="222330528"/>
+        <c:axId val="222328960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208716432"/>
+        <c:axId val="222330528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2036,7 +2045,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208715256"/>
+        <c:crossAx val="222328960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2044,7 +2053,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208715256"/>
+        <c:axId val="222328960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2110,7 +2119,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208716432"/>
+        <c:crossAx val="222330528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2289,11 +2298,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="208715648"/>
-        <c:axId val="208717608"/>
+        <c:axId val="222333272"/>
+        <c:axId val="222327784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208715648"/>
+        <c:axId val="222333272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2350,7 +2359,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208717608"/>
+        <c:crossAx val="222327784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2358,7 +2367,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208717608"/>
+        <c:axId val="222327784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2424,7 +2433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208715648"/>
+        <c:crossAx val="222333272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2603,11 +2612,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="209286800"/>
-        <c:axId val="209292288"/>
+        <c:axId val="222329352"/>
+        <c:axId val="222329744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209286800"/>
+        <c:axId val="222329352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2664,7 +2673,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209292288"/>
+        <c:crossAx val="222329744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2672,7 +2681,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209292288"/>
+        <c:axId val="222329744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2738,7 +2747,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209286800"/>
+        <c:crossAx val="222329352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2917,11 +2926,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="209286408"/>
-        <c:axId val="209287192"/>
+        <c:axId val="222334056"/>
+        <c:axId val="223897928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209286408"/>
+        <c:axId val="222334056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2978,7 +2987,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209287192"/>
+        <c:crossAx val="223897928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2986,7 +2995,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209287192"/>
+        <c:axId val="223897928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3052,7 +3061,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209286408"/>
+        <c:crossAx val="222334056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3105,7 +3114,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3146,7 +3155,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3187,7 +3196,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3228,7 +3237,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3269,7 +3278,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3310,7 +3319,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3351,7 +3360,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5428,8 +5437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5532,7 +5541,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5547,7 +5556,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5565,7 +5574,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5583,7 +5592,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5601,7 +5610,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5619,11 +5628,11 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -5641,7 +5650,7 @@
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
@@ -5917,21 +5926,35 @@
       <c r="A30" s="1">
         <v>14</v>
       </c>
-      <c r="B30" s="35"/>
+      <c r="B30" s="35" t="s">
+        <v>30</v>
+      </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="37"/>
+      <c r="D30" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>150</v>
+      </c>
       <c r="F30" s="38"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>15</v>
       </c>
-      <c r="B31" s="35"/>
+      <c r="B31" s="35" t="s">
+        <v>30</v>
+      </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="38"/>
+      <c r="D31" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="E31" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="F31" s="38" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">

</xml_diff>

<commit_message>
P05 Add Customer equals(Object o) revisions to GitHub
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="157">
   <si>
     <t>Product Name:</t>
   </si>
@@ -509,6 +509,9 @@
   </si>
   <si>
     <t>Add Customer REGEX revisions to GitHub</t>
+  </si>
+  <si>
+    <t>Add Customer equals(Object o) revisions to GitHub</t>
   </si>
 </sst>
 </file>
@@ -900,6 +903,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1074,6 +1078,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1146,6 +1151,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1237,6 +1243,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1307,22 +1314,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5</c:v>
@@ -1386,6 +1393,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1460,6 +1468,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3684,7 +3693,7 @@
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5437,8 +5446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5541,7 +5550,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5556,7 +5565,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5574,7 +5583,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5592,7 +5601,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5610,7 +5619,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5628,7 +5637,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5650,7 +5659,7 @@
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
@@ -5960,11 +5969,19 @@
       <c r="A32" s="1">
         <v>16</v>
       </c>
-      <c r="B32" s="35"/>
+      <c r="B32" s="35" t="s">
+        <v>30</v>
+      </c>
       <c r="C32" s="1"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="38"/>
+      <c r="D32" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="F32" s="38" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1">

</xml_diff>

<commit_message>
P05 Add Option equals(Object o) revisions to GitHub
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="158">
   <si>
     <t>Product Name:</t>
   </si>
@@ -512,6 +512,9 @@
   </si>
   <si>
     <t>Add Customer equals(Object o) revisions to GitHub</t>
+  </si>
+  <si>
+    <t>Add neg., throw IllegalArgumentException Option to GitHub</t>
   </si>
 </sst>
 </file>
@@ -903,7 +906,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1046,11 +1048,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="222334448"/>
-        <c:axId val="222331704"/>
+        <c:axId val="164049472"/>
+        <c:axId val="108067560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="222334448"/>
+        <c:axId val="164049472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1078,7 +1080,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1110,12 +1111,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222331704"/>
+        <c:crossAx val="108067560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="222331704"/>
+        <c:axId val="108067560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1151,7 +1152,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1183,7 +1183,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222334448"/>
+        <c:crossAx val="164049472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1243,7 +1243,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1314,28 +1313,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1363,11 +1362,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="222332096"/>
-        <c:axId val="222332880"/>
+        <c:axId val="209670448"/>
+        <c:axId val="164339544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="222332096"/>
+        <c:axId val="209670448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1393,7 +1392,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1425,7 +1423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222332880"/>
+        <c:crossAx val="164339544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1433,7 +1431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222332880"/>
+        <c:axId val="164339544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1468,7 +1466,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1500,7 +1497,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222332096"/>
+        <c:crossAx val="209670448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1679,11 +1676,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="222331312"/>
-        <c:axId val="222333664"/>
+        <c:axId val="210051120"/>
+        <c:axId val="210051512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="222331312"/>
+        <c:axId val="210051120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1740,7 +1737,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222333664"/>
+        <c:crossAx val="210051512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1748,7 +1745,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222333664"/>
+        <c:axId val="210051512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1814,7 +1811,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222331312"/>
+        <c:crossAx val="210051120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1993,11 +1990,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="222330528"/>
-        <c:axId val="222328960"/>
+        <c:axId val="210057000"/>
+        <c:axId val="210051904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="222330528"/>
+        <c:axId val="210057000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2054,7 +2051,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222328960"/>
+        <c:crossAx val="210051904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2062,7 +2059,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222328960"/>
+        <c:axId val="210051904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2128,7 +2125,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222330528"/>
+        <c:crossAx val="210057000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2307,11 +2304,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="222333272"/>
-        <c:axId val="222327784"/>
+        <c:axId val="210053080"/>
+        <c:axId val="210053864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="222333272"/>
+        <c:axId val="210053080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2368,7 +2365,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222327784"/>
+        <c:crossAx val="210053864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2376,7 +2373,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222327784"/>
+        <c:axId val="210053864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2442,7 +2439,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222333272"/>
+        <c:crossAx val="210053080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2621,11 +2618,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="222329352"/>
-        <c:axId val="222329744"/>
+        <c:axId val="210054256"/>
+        <c:axId val="210058176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="222329352"/>
+        <c:axId val="210054256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2682,7 +2679,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222329744"/>
+        <c:crossAx val="210058176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2690,7 +2687,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222329744"/>
+        <c:axId val="210058176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2756,7 +2753,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222329352"/>
+        <c:crossAx val="210054256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2935,11 +2932,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="222334056"/>
-        <c:axId val="223897928"/>
+        <c:axId val="210055824"/>
+        <c:axId val="210056216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="222334056"/>
+        <c:axId val="210055824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2996,7 +2993,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223897928"/>
+        <c:crossAx val="210056216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3004,7 +3001,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="223897928"/>
+        <c:axId val="210056216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3070,7 +3067,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222334056"/>
+        <c:crossAx val="210055824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5446,8 +5443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5550,7 +5547,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5565,7 +5562,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5583,7 +5580,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5601,7 +5598,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5619,7 +5616,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5637,7 +5634,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5655,11 +5652,11 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
@@ -5673,7 +5670,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -5992,20 +5989,30 @@
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="E33" s="37"/>
+        <v>157</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>154</v>
+      </c>
       <c r="F33" s="38"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>18</v>
       </c>
-      <c r="B34" s="35"/>
+      <c r="B34" s="35" t="s">
+        <v>35</v>
+      </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="38"/>
+      <c r="D34" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="F34" s="38" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">

</xml_diff>

<commit_message>
P05 Add Computer equals(Object o) revisions to GitHub
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="161">
   <si>
     <t>Product Name:</t>
   </si>
@@ -515,6 +515,15 @@
   </si>
   <si>
     <t>Add neg., throw IllegalArgumentException Option to GitHub</t>
+  </si>
+  <si>
+    <t>Add Option equals(Object o) revisions to GitHub</t>
+  </si>
+  <si>
+    <t>Completed Day 7</t>
+  </si>
+  <si>
+    <t>Add Computer equals(Object o) revisions to GitHub</t>
   </si>
 </sst>
 </file>
@@ -906,6 +915,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1080,6 +1090,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1152,6 +1163,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1313,25 +1325,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>5</c:v>
@@ -3690,7 +3702,7 @@
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5443,8 +5455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5547,7 +5559,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5562,7 +5574,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5580,7 +5592,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5598,7 +5610,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5616,7 +5628,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5634,7 +5646,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5652,7 +5664,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5674,7 +5686,7 @@
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
@@ -6005,7 +6017,7 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="39" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E34" s="37" t="s">
         <v>154</v>
@@ -6018,11 +6030,19 @@
       <c r="A35" s="1">
         <v>19</v>
       </c>
-      <c r="B35" s="35"/>
+      <c r="B35" s="35" t="s">
+        <v>40</v>
+      </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="38"/>
+      <c r="D35" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="F35" s="38" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">

</xml_diff>

<commit_message>
P05 Add Store to GitHub
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="163">
   <si>
     <t>Product Name:</t>
   </si>
@@ -524,6 +524,12 @@
   </si>
   <si>
     <t>Add Computer equals(Object o) revisions to GitHub</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 6</t>
+  </si>
+  <si>
+    <t>Add Store to GitHub</t>
   </si>
 </sst>
 </file>
@@ -1255,6 +1261,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1325,28 +1332,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1404,6 +1411,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1478,6 +1486,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3701,8 +3710,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4135,7 +4144,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="H24" s="18" t="s">
         <v>31</v>
@@ -4168,7 +4177,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="H25" s="18" t="s">
         <v>36</v>
@@ -4200,7 +4209,9 @@
       <c r="F26" s="17">
         <v>1</v>
       </c>
-      <c r="G26" s="17"/>
+      <c r="G26" s="17" t="s">
+        <v>138</v>
+      </c>
       <c r="H26" s="18" t="s">
         <v>31</v>
       </c>
@@ -4230,7 +4241,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="H27" s="18" t="s">
         <v>31</v>
@@ -4260,7 +4271,9 @@
       <c r="F28" s="17">
         <v>1</v>
       </c>
-      <c r="G28" s="17"/>
+      <c r="G28" s="17" t="s">
+        <v>138</v>
+      </c>
       <c r="H28" s="18" t="s">
         <v>31</v>
       </c>
@@ -5455,8 +5468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5559,7 +5572,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5574,7 +5587,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5592,7 +5605,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5610,7 +5623,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5628,7 +5641,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5646,7 +5659,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5664,7 +5677,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5682,7 +5695,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -6048,10 +6061,16 @@
       <c r="A36" s="1">
         <v>20</v>
       </c>
-      <c r="B36" s="35"/>
+      <c r="B36" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="37"/>
+      <c r="D36" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="E36" s="37" t="s">
+        <v>138</v>
+      </c>
       <c r="F36" s="38"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
P05 Add TestStore to GitHub
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="164">
   <si>
     <t>Product Name:</t>
   </si>
@@ -530,6 +530,9 @@
   </si>
   <si>
     <t>Add Store to GitHub</t>
+  </si>
+  <si>
+    <t>Add TestStore to GitHub</t>
   </si>
 </sst>
 </file>
@@ -1332,28 +1335,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3710,8 +3713,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5468,8 +5471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5572,7 +5575,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5587,7 +5590,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5605,7 +5608,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5623,7 +5626,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5641,7 +5644,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5659,7 +5662,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5677,7 +5680,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5695,7 +5698,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -6077,10 +6080,16 @@
       <c r="A37" s="1">
         <v>21</v>
       </c>
-      <c r="B37" s="35"/>
+      <c r="B37" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="37"/>
+      <c r="D37" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="E37" s="37" t="s">
+        <v>138</v>
+      </c>
       <c r="F37" s="38"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
P05 NO data diplayed ~ java TestStore
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="166">
   <si>
     <t>Product Name:</t>
   </si>
@@ -533,6 +533,12 @@
   </si>
   <si>
     <t>Add TestStore to GitHub</t>
+  </si>
+  <si>
+    <t>TestStore completed</t>
+  </si>
+  <si>
+    <t>NO data displayed ~ java TestStore</t>
   </si>
 </sst>
 </file>
@@ -1335,25 +1341,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
@@ -5472,7 +5478,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5575,7 +5581,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5590,7 +5596,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5608,7 +5614,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5626,7 +5632,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5644,7 +5650,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5662,7 +5668,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5680,7 +5686,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5702,7 +5708,7 @@
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
@@ -6096,11 +6102,19 @@
       <c r="A38" s="1">
         <v>22</v>
       </c>
-      <c r="B38" s="35"/>
+      <c r="B38" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="38"/>
+      <c r="D38" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="E38" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="F38" s="38" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1">

</xml_diff>